<commit_message>
updated mid atlantic plotting
</commit_message>
<xml_diff>
--- a/projects/mid_atlantic/fixed_depth_monte_carlo/user_inputs_fixed_depth_monte_carlo.xlsx
+++ b/projects/mid_atlantic/fixed_depth_monte_carlo/user_inputs_fixed_depth_monte_carlo.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23029"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2B3BA04-EE35-4359-888E-6D1FBFF3352D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40218607-CB76-48E2-A080-467780E3C1EE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="656" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="656" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="fixed_diameter" sheetId="10" r:id="rId1"/>
@@ -532,8 +532,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{33148202-7FD3-419C-810B-5ECE05747F7D}">
   <dimension ref="A1:H29"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:D2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -687,7 +687,7 @@
         <v>8</v>
       </c>
       <c r="E6" s="8">
-        <v>1</v>
+        <v>100</v>
       </c>
       <c r="F6" s="8">
         <v>650</v>
@@ -713,10 +713,10 @@
         <v>8</v>
       </c>
       <c r="E7" s="8">
-        <v>5</v>
+        <v>50</v>
       </c>
       <c r="F7" s="8">
-        <v>550</v>
+        <v>150</v>
       </c>
       <c r="G7" s="8">
         <v>0</v>
@@ -1305,8 +1305,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:D2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E6" sqref="E6:F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1460,7 +1460,7 @@
         <v>8</v>
       </c>
       <c r="E6" s="8">
-        <v>1</v>
+        <v>100</v>
       </c>
       <c r="F6" s="8">
         <v>650</v>
@@ -1486,10 +1486,10 @@
         <v>8</v>
       </c>
       <c r="E7" s="8">
-        <v>5</v>
+        <v>50</v>
       </c>
       <c r="F7" s="8">
-        <v>550</v>
+        <v>150</v>
       </c>
       <c r="G7" s="8">
         <v>0</v>

</xml_diff>